<commit_message>
edit paragraph and word
</commit_message>
<xml_diff>
--- a/assignment1/ListWord.xlsx
+++ b/assignment1/ListWord.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuipied-my.sharepoint.com/personal/thammasat_tho_dome_tu_ac_th/Documents/CN332/CN332-Default/assignment1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="8_{D941D1B1-9613-1745-9C37-F2C7619A9AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{787122C0-E429-A548-B2F5-75F7514CC4F2}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="8_{D941D1B1-9613-1745-9C37-F2C7619A9AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{470A8571-A063-AA43-A5B9-0D17552CF317}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="780" windowWidth="28040" windowHeight="17300" xr2:uid="{722068D7-275B-C542-BB87-59CC7BFD0B28}"/>
+    <workbookView xWindow="1100" yWindow="760" windowWidth="28040" windowHeight="17200" xr2:uid="{722068D7-275B-C542-BB87-59CC7BFD0B28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -527,12 +527,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -540,38 +539,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1448,7 +1416,728 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B75C37E0-2A1E-C343-B204-497458A3F342}" name="PivotTable5" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A55E039D-19CF-B847-8840-91207B73EC0C}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="H1:I50" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="73">
+        <item x="42"/>
+        <item x="33"/>
+        <item x="67"/>
+        <item x="22"/>
+        <item x="9"/>
+        <item x="58"/>
+        <item x="52"/>
+        <item x="14"/>
+        <item x="19"/>
+        <item x="2"/>
+        <item x="32"/>
+        <item x="57"/>
+        <item x="21"/>
+        <item x="11"/>
+        <item x="45"/>
+        <item x="59"/>
+        <item x="54"/>
+        <item x="37"/>
+        <item x="36"/>
+        <item x="41"/>
+        <item x="20"/>
+        <item x="69"/>
+        <item x="13"/>
+        <item x="66"/>
+        <item x="25"/>
+        <item x="28"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="10"/>
+        <item x="68"/>
+        <item x="62"/>
+        <item x="31"/>
+        <item x="38"/>
+        <item x="40"/>
+        <item x="26"/>
+        <item x="44"/>
+        <item x="24"/>
+        <item x="70"/>
+        <item x="47"/>
+        <item x="43"/>
+        <item x="60"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="46"/>
+        <item x="63"/>
+        <item x="29"/>
+        <item x="49"/>
+        <item x="35"/>
+        <item x="27"/>
+        <item x="61"/>
+        <item x="23"/>
+        <item x="0"/>
+        <item x="64"/>
+        <item x="34"/>
+        <item x="7"/>
+        <item x="17"/>
+        <item x="3"/>
+        <item x="51"/>
+        <item x="30"/>
+        <item x="48"/>
+        <item x="53"/>
+        <item x="6"/>
+        <item x="18"/>
+        <item x="1"/>
+        <item x="50"/>
+        <item x="16"/>
+        <item x="39"/>
+        <item x="12"/>
+        <item x="15"/>
+        <item x="8"/>
+        <item x="65"/>
+        <item x="71"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0">
+      <items count="50">
+        <item x="44"/>
+        <item x="43"/>
+        <item x="41"/>
+        <item x="11"/>
+        <item x="0"/>
+        <item x="24"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="38"/>
+        <item x="21"/>
+        <item x="33"/>
+        <item x="20"/>
+        <item x="6"/>
+        <item x="19"/>
+        <item x="45"/>
+        <item x="40"/>
+        <item x="42"/>
+        <item x="36"/>
+        <item x="17"/>
+        <item x="2"/>
+        <item x="22"/>
+        <item x="29"/>
+        <item x="4"/>
+        <item x="31"/>
+        <item x="12"/>
+        <item x="28"/>
+        <item x="8"/>
+        <item x="35"/>
+        <item x="10"/>
+        <item x="27"/>
+        <item x="15"/>
+        <item x="34"/>
+        <item x="14"/>
+        <item x="13"/>
+        <item x="23"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item x="30"/>
+        <item x="26"/>
+        <item x="47"/>
+        <item x="39"/>
+        <item x="32"/>
+        <item x="16"/>
+        <item x="3"/>
+        <item x="46"/>
+        <item x="25"/>
+        <item x="37"/>
+        <item x="18"/>
+        <item h="1" x="48"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="16">
+        <item x="3"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="12"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="11"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="14"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="49">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Verb" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DB74C30F-8590-6E4B-B43E-2107187265E9}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="E1:F73" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0">
+      <items count="73">
+        <item x="42"/>
+        <item x="33"/>
+        <item x="67"/>
+        <item x="22"/>
+        <item x="9"/>
+        <item x="58"/>
+        <item x="52"/>
+        <item x="14"/>
+        <item x="19"/>
+        <item x="2"/>
+        <item x="32"/>
+        <item x="57"/>
+        <item x="21"/>
+        <item x="11"/>
+        <item x="45"/>
+        <item x="59"/>
+        <item x="54"/>
+        <item x="37"/>
+        <item x="36"/>
+        <item x="41"/>
+        <item x="20"/>
+        <item x="69"/>
+        <item x="13"/>
+        <item x="66"/>
+        <item x="25"/>
+        <item x="28"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="10"/>
+        <item x="68"/>
+        <item x="62"/>
+        <item x="31"/>
+        <item x="38"/>
+        <item x="40"/>
+        <item x="26"/>
+        <item x="44"/>
+        <item x="24"/>
+        <item x="70"/>
+        <item x="47"/>
+        <item x="43"/>
+        <item x="60"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="46"/>
+        <item x="63"/>
+        <item x="29"/>
+        <item x="49"/>
+        <item x="35"/>
+        <item x="27"/>
+        <item x="61"/>
+        <item x="23"/>
+        <item x="0"/>
+        <item x="64"/>
+        <item x="34"/>
+        <item x="7"/>
+        <item x="17"/>
+        <item x="3"/>
+        <item x="51"/>
+        <item x="30"/>
+        <item x="48"/>
+        <item x="53"/>
+        <item x="6"/>
+        <item x="18"/>
+        <item x="1"/>
+        <item x="50"/>
+        <item x="16"/>
+        <item x="39"/>
+        <item x="12"/>
+        <item x="15"/>
+        <item x="8"/>
+        <item x="65"/>
+        <item h="1" x="71"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="50">
+        <item x="44"/>
+        <item x="43"/>
+        <item x="41"/>
+        <item x="11"/>
+        <item x="0"/>
+        <item x="24"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="38"/>
+        <item x="21"/>
+        <item x="33"/>
+        <item x="20"/>
+        <item x="6"/>
+        <item x="19"/>
+        <item x="45"/>
+        <item x="40"/>
+        <item x="42"/>
+        <item x="36"/>
+        <item x="17"/>
+        <item x="2"/>
+        <item x="22"/>
+        <item x="29"/>
+        <item x="4"/>
+        <item x="31"/>
+        <item x="12"/>
+        <item x="28"/>
+        <item x="8"/>
+        <item x="35"/>
+        <item x="10"/>
+        <item x="27"/>
+        <item x="15"/>
+        <item x="34"/>
+        <item x="14"/>
+        <item x="13"/>
+        <item x="23"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item x="30"/>
+        <item x="26"/>
+        <item x="47"/>
+        <item x="39"/>
+        <item x="32"/>
+        <item x="16"/>
+        <item x="3"/>
+        <item x="46"/>
+        <item x="25"/>
+        <item x="37"/>
+        <item x="18"/>
+        <item x="48"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="16">
+        <item x="3"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="12"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="11"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="14"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="72">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="49"/>
+    </i>
+    <i>
+      <x v="50"/>
+    </i>
+    <i>
+      <x v="51"/>
+    </i>
+    <i>
+      <x v="52"/>
+    </i>
+    <i>
+      <x v="53"/>
+    </i>
+    <i>
+      <x v="54"/>
+    </i>
+    <i>
+      <x v="55"/>
+    </i>
+    <i>
+      <x v="56"/>
+    </i>
+    <i>
+      <x v="57"/>
+    </i>
+    <i>
+      <x v="58"/>
+    </i>
+    <i>
+      <x v="59"/>
+    </i>
+    <i>
+      <x v="60"/>
+    </i>
+    <i>
+      <x v="61"/>
+    </i>
+    <i>
+      <x v="62"/>
+    </i>
+    <i>
+      <x v="63"/>
+    </i>
+    <i>
+      <x v="64"/>
+    </i>
+    <i>
+      <x v="65"/>
+    </i>
+    <i>
+      <x v="66"/>
+    </i>
+    <i>
+      <x v="67"/>
+    </i>
+    <i>
+      <x v="68"/>
+    </i>
+    <i>
+      <x v="69"/>
+    </i>
+    <i>
+      <x v="70"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Noun" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B75C37E0-2A1E-C343-B204-497458A3F342}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="N5:P6" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="3">
     <pivotField dataField="1" compact="0" outline="0" showAll="0">
@@ -1637,8 +2326,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E4B67667-F814-4D48-8D57-36D60A9AB9F3}" name="PivotTable4" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E4B67667-F814-4D48-8D57-36D60A9AB9F3}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="K1:L16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField compact="0" outline="0" showAll="0">
@@ -1848,727 +2537,6 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Count of Adjective" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A55E039D-19CF-B847-8840-91207B73EC0C}" name="PivotTable3" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="H1:I50" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="73">
-        <item x="42"/>
-        <item x="33"/>
-        <item x="67"/>
-        <item x="22"/>
-        <item x="9"/>
-        <item x="58"/>
-        <item x="52"/>
-        <item x="14"/>
-        <item x="19"/>
-        <item x="2"/>
-        <item x="32"/>
-        <item x="57"/>
-        <item x="21"/>
-        <item x="11"/>
-        <item x="45"/>
-        <item x="59"/>
-        <item x="54"/>
-        <item x="37"/>
-        <item x="36"/>
-        <item x="41"/>
-        <item x="20"/>
-        <item x="69"/>
-        <item x="13"/>
-        <item x="66"/>
-        <item x="25"/>
-        <item x="28"/>
-        <item x="55"/>
-        <item x="56"/>
-        <item x="10"/>
-        <item x="68"/>
-        <item x="62"/>
-        <item x="31"/>
-        <item x="38"/>
-        <item x="40"/>
-        <item x="26"/>
-        <item x="44"/>
-        <item x="24"/>
-        <item x="70"/>
-        <item x="47"/>
-        <item x="43"/>
-        <item x="60"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="46"/>
-        <item x="63"/>
-        <item x="29"/>
-        <item x="49"/>
-        <item x="35"/>
-        <item x="27"/>
-        <item x="61"/>
-        <item x="23"/>
-        <item x="0"/>
-        <item x="64"/>
-        <item x="34"/>
-        <item x="7"/>
-        <item x="17"/>
-        <item x="3"/>
-        <item x="51"/>
-        <item x="30"/>
-        <item x="48"/>
-        <item x="53"/>
-        <item x="6"/>
-        <item x="18"/>
-        <item x="1"/>
-        <item x="50"/>
-        <item x="16"/>
-        <item x="39"/>
-        <item x="12"/>
-        <item x="15"/>
-        <item x="8"/>
-        <item x="65"/>
-        <item x="71"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0">
-      <items count="50">
-        <item x="44"/>
-        <item x="43"/>
-        <item x="41"/>
-        <item x="11"/>
-        <item x="0"/>
-        <item x="24"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="38"/>
-        <item x="21"/>
-        <item x="33"/>
-        <item x="20"/>
-        <item x="6"/>
-        <item x="19"/>
-        <item x="45"/>
-        <item x="40"/>
-        <item x="42"/>
-        <item x="36"/>
-        <item x="17"/>
-        <item x="2"/>
-        <item x="22"/>
-        <item x="29"/>
-        <item x="4"/>
-        <item x="31"/>
-        <item x="12"/>
-        <item x="28"/>
-        <item x="8"/>
-        <item x="35"/>
-        <item x="10"/>
-        <item x="27"/>
-        <item x="15"/>
-        <item x="34"/>
-        <item x="14"/>
-        <item x="13"/>
-        <item x="23"/>
-        <item x="9"/>
-        <item x="7"/>
-        <item x="30"/>
-        <item x="26"/>
-        <item x="47"/>
-        <item x="39"/>
-        <item x="32"/>
-        <item x="16"/>
-        <item x="3"/>
-        <item x="46"/>
-        <item x="25"/>
-        <item x="37"/>
-        <item x="18"/>
-        <item h="1" x="48"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="16">
-        <item x="3"/>
-        <item x="2"/>
-        <item x="8"/>
-        <item x="1"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="12"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="11"/>
-        <item x="0"/>
-        <item x="13"/>
-        <item x="4"/>
-        <item x="6"/>
-        <item x="14"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="49">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="33"/>
-    </i>
-    <i>
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="35"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="39"/>
-    </i>
-    <i>
-      <x v="40"/>
-    </i>
-    <i>
-      <x v="41"/>
-    </i>
-    <i>
-      <x v="42"/>
-    </i>
-    <i>
-      <x v="43"/>
-    </i>
-    <i>
-      <x v="44"/>
-    </i>
-    <i>
-      <x v="45"/>
-    </i>
-    <i>
-      <x v="46"/>
-    </i>
-    <i>
-      <x v="47"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Verb" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DB74C30F-8590-6E4B-B43E-2107187265E9}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="E1:F73" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0">
-      <items count="73">
-        <item x="42"/>
-        <item x="33"/>
-        <item x="67"/>
-        <item x="22"/>
-        <item x="9"/>
-        <item x="58"/>
-        <item x="52"/>
-        <item x="14"/>
-        <item x="19"/>
-        <item x="2"/>
-        <item x="32"/>
-        <item x="57"/>
-        <item x="21"/>
-        <item x="11"/>
-        <item x="45"/>
-        <item x="59"/>
-        <item x="54"/>
-        <item x="37"/>
-        <item x="36"/>
-        <item x="41"/>
-        <item x="20"/>
-        <item x="69"/>
-        <item x="13"/>
-        <item x="66"/>
-        <item x="25"/>
-        <item x="28"/>
-        <item x="55"/>
-        <item x="56"/>
-        <item x="10"/>
-        <item x="68"/>
-        <item x="62"/>
-        <item x="31"/>
-        <item x="38"/>
-        <item x="40"/>
-        <item x="26"/>
-        <item x="44"/>
-        <item x="24"/>
-        <item x="70"/>
-        <item x="47"/>
-        <item x="43"/>
-        <item x="60"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="46"/>
-        <item x="63"/>
-        <item x="29"/>
-        <item x="49"/>
-        <item x="35"/>
-        <item x="27"/>
-        <item x="61"/>
-        <item x="23"/>
-        <item x="0"/>
-        <item x="64"/>
-        <item x="34"/>
-        <item x="7"/>
-        <item x="17"/>
-        <item x="3"/>
-        <item x="51"/>
-        <item x="30"/>
-        <item x="48"/>
-        <item x="53"/>
-        <item x="6"/>
-        <item x="18"/>
-        <item x="1"/>
-        <item x="50"/>
-        <item x="16"/>
-        <item x="39"/>
-        <item x="12"/>
-        <item x="15"/>
-        <item x="8"/>
-        <item x="65"/>
-        <item h="1" x="71"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="50">
-        <item x="44"/>
-        <item x="43"/>
-        <item x="41"/>
-        <item x="11"/>
-        <item x="0"/>
-        <item x="24"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="38"/>
-        <item x="21"/>
-        <item x="33"/>
-        <item x="20"/>
-        <item x="6"/>
-        <item x="19"/>
-        <item x="45"/>
-        <item x="40"/>
-        <item x="42"/>
-        <item x="36"/>
-        <item x="17"/>
-        <item x="2"/>
-        <item x="22"/>
-        <item x="29"/>
-        <item x="4"/>
-        <item x="31"/>
-        <item x="12"/>
-        <item x="28"/>
-        <item x="8"/>
-        <item x="35"/>
-        <item x="10"/>
-        <item x="27"/>
-        <item x="15"/>
-        <item x="34"/>
-        <item x="14"/>
-        <item x="13"/>
-        <item x="23"/>
-        <item x="9"/>
-        <item x="7"/>
-        <item x="30"/>
-        <item x="26"/>
-        <item x="47"/>
-        <item x="39"/>
-        <item x="32"/>
-        <item x="16"/>
-        <item x="3"/>
-        <item x="46"/>
-        <item x="25"/>
-        <item x="37"/>
-        <item x="18"/>
-        <item x="48"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0">
-      <items count="16">
-        <item x="3"/>
-        <item x="2"/>
-        <item x="8"/>
-        <item x="1"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="12"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="11"/>
-        <item x="0"/>
-        <item x="13"/>
-        <item x="4"/>
-        <item x="6"/>
-        <item x="14"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="72">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="33"/>
-    </i>
-    <i>
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="35"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="39"/>
-    </i>
-    <i>
-      <x v="40"/>
-    </i>
-    <i>
-      <x v="41"/>
-    </i>
-    <i>
-      <x v="42"/>
-    </i>
-    <i>
-      <x v="43"/>
-    </i>
-    <i>
-      <x v="44"/>
-    </i>
-    <i>
-      <x v="45"/>
-    </i>
-    <i>
-      <x v="46"/>
-    </i>
-    <i>
-      <x v="47"/>
-    </i>
-    <i>
-      <x v="48"/>
-    </i>
-    <i>
-      <x v="49"/>
-    </i>
-    <i>
-      <x v="50"/>
-    </i>
-    <i>
-      <x v="51"/>
-    </i>
-    <i>
-      <x v="52"/>
-    </i>
-    <i>
-      <x v="53"/>
-    </i>
-    <i>
-      <x v="54"/>
-    </i>
-    <i>
-      <x v="55"/>
-    </i>
-    <i>
-      <x v="56"/>
-    </i>
-    <i>
-      <x v="57"/>
-    </i>
-    <i>
-      <x v="58"/>
-    </i>
-    <i>
-      <x v="59"/>
-    </i>
-    <i>
-      <x v="60"/>
-    </i>
-    <i>
-      <x v="61"/>
-    </i>
-    <i>
-      <x v="62"/>
-    </i>
-    <i>
-      <x v="63"/>
-    </i>
-    <i>
-      <x v="64"/>
-    </i>
-    <i>
-      <x v="65"/>
-    </i>
-    <i>
-      <x v="66"/>
-    </i>
-    <i>
-      <x v="67"/>
-    </i>
-    <i>
-      <x v="68"/>
-    </i>
-    <i>
-      <x v="69"/>
-    </i>
-    <i>
-      <x v="70"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Noun" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -2902,8 +2870,8 @@
   <dimension ref="A1:P140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N23" sqref="N23"/>
+      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M18" sqref="M18:R43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3168,11 +3136,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3205,19 +3173,19 @@
       <c r="E2" t="s">
         <v>107</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2">
         <v>1</v>
       </c>
       <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2">
         <v>1</v>
       </c>
     </row>
@@ -3234,19 +3202,19 @@
       <c r="E3" t="s">
         <v>98</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3">
         <v>1</v>
       </c>
       <c r="K3" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3">
         <v>1</v>
       </c>
     </row>
@@ -3263,19 +3231,19 @@
       <c r="E4" t="s">
         <v>131</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4">
         <v>1</v>
       </c>
       <c r="H4" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4">
         <v>1</v>
       </c>
       <c r="K4" t="s">
         <v>58</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4">
         <v>1</v>
       </c>
     </row>
@@ -3292,19 +3260,19 @@
       <c r="E5" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5">
         <v>1</v>
       </c>
       <c r="K5" t="s">
         <v>52</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5">
         <v>1</v>
       </c>
       <c r="N5" t="s">
@@ -3330,28 +3298,28 @@
       <c r="E6" t="s">
         <v>74</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6">
         <v>5</v>
       </c>
       <c r="H6" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6">
         <v>1</v>
       </c>
       <c r="K6" t="s">
         <v>59</v>
       </c>
-      <c r="L6" s="4">
-        <v>1</v>
-      </c>
-      <c r="N6" s="4">
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="N6">
         <v>138</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6">
         <v>58</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6">
         <v>15</v>
       </c>
     </row>
@@ -3368,19 +3336,19 @@
       <c r="E7" t="s">
         <v>122</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7">
         <v>1</v>
       </c>
       <c r="H7" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7">
         <v>1</v>
       </c>
       <c r="K7" t="s">
         <v>60</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7">
         <v>1</v>
       </c>
     </row>
@@ -3397,19 +3365,19 @@
       <c r="E8" t="s">
         <v>116</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8">
         <v>1</v>
       </c>
       <c r="H8" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8">
         <v>1</v>
       </c>
       <c r="K8" t="s">
         <v>62</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8">
         <v>2</v>
       </c>
     </row>
@@ -3426,19 +3394,19 @@
       <c r="E9" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9">
         <v>1</v>
       </c>
       <c r="H9" t="s">
         <v>4</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9">
         <v>2</v>
       </c>
       <c r="K9" t="s">
         <v>55</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9">
         <v>1</v>
       </c>
     </row>
@@ -3455,19 +3423,19 @@
       <c r="E10" t="s">
         <v>83</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10">
         <v>6</v>
       </c>
       <c r="H10" t="s">
         <v>41</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10">
         <v>1</v>
       </c>
       <c r="K10" t="s">
         <v>57</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10">
         <v>1</v>
       </c>
     </row>
@@ -3484,19 +3452,19 @@
       <c r="E11" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11">
         <v>4</v>
       </c>
       <c r="H11" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11">
         <v>1</v>
       </c>
       <c r="K11" t="s">
         <v>61</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11">
         <v>1</v>
       </c>
     </row>
@@ -3513,19 +3481,19 @@
       <c r="E12" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12">
         <v>1</v>
       </c>
       <c r="H12" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12">
         <v>1</v>
       </c>
       <c r="K12" t="s">
         <v>51</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12">
         <v>1</v>
       </c>
     </row>
@@ -3542,19 +3510,19 @@
       <c r="E13" t="s">
         <v>121</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13">
         <v>1</v>
       </c>
       <c r="H13" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13">
         <v>1</v>
       </c>
       <c r="K13" t="s">
         <v>63</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13">
         <v>1</v>
       </c>
     </row>
@@ -3571,19 +3539,19 @@
       <c r="E14" t="s">
         <v>85</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14">
         <v>2</v>
       </c>
       <c r="H14" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14">
         <v>1</v>
       </c>
       <c r="K14" t="s">
         <v>54</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14">
         <v>1</v>
       </c>
     </row>
@@ -3600,19 +3568,19 @@
       <c r="E15" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15">
         <v>4</v>
       </c>
       <c r="H15" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15">
         <v>2</v>
       </c>
       <c r="K15" t="s">
         <v>56</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15">
         <v>1</v>
       </c>
     </row>
@@ -3629,19 +3597,19 @@
       <c r="E16" t="s">
         <v>109</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16">
         <v>4</v>
       </c>
       <c r="H16" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16">
         <v>2</v>
       </c>
       <c r="K16" t="s">
         <v>138</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16">
         <v>15</v>
       </c>
     </row>
@@ -3658,13 +3626,13 @@
       <c r="E17" t="s">
         <v>123</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17">
         <v>1</v>
       </c>
       <c r="H17" t="s">
         <v>43</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17">
         <v>1</v>
       </c>
     </row>
@@ -3678,13 +3646,13 @@
       <c r="E18" t="s">
         <v>118</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18">
         <v>2</v>
       </c>
       <c r="H18" t="s">
         <v>45</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18">
         <v>1</v>
       </c>
     </row>
@@ -3698,13 +3666,13 @@
       <c r="E19" t="s">
         <v>102</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19">
         <v>1</v>
       </c>
       <c r="H19" t="s">
         <v>39</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19">
         <v>1</v>
       </c>
     </row>
@@ -3718,13 +3686,13 @@
       <c r="E20" t="s">
         <v>101</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20">
         <v>1</v>
       </c>
       <c r="H20" t="s">
         <v>20</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20">
         <v>1</v>
       </c>
     </row>
@@ -3738,13 +3706,13 @@
       <c r="E21" t="s">
         <v>106</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21">
         <v>1</v>
       </c>
       <c r="H21" t="s">
         <v>5</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21">
         <v>1</v>
       </c>
     </row>
@@ -3758,13 +3726,13 @@
       <c r="E22" t="s">
         <v>84</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22">
         <v>2</v>
       </c>
       <c r="H22" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22">
         <v>1</v>
       </c>
     </row>
@@ -3778,13 +3746,13 @@
       <c r="E23" t="s">
         <v>137</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23">
         <v>1</v>
       </c>
       <c r="H23" t="s">
         <v>32</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23">
         <v>2</v>
       </c>
     </row>
@@ -3798,13 +3766,13 @@
       <c r="E24" t="s">
         <v>78</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24">
         <v>3</v>
       </c>
       <c r="H24" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I24">
         <v>3</v>
       </c>
     </row>
@@ -3818,13 +3786,13 @@
       <c r="E25" t="s">
         <v>130</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25">
         <v>1</v>
       </c>
       <c r="H25" t="s">
         <v>34</v>
       </c>
-      <c r="I25" s="4">
+      <c r="I25">
         <v>1</v>
       </c>
     </row>
@@ -3838,13 +3806,13 @@
       <c r="E26" t="s">
         <v>89</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26">
         <v>1</v>
       </c>
       <c r="H26" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="4">
+      <c r="I26">
         <v>1</v>
       </c>
     </row>
@@ -3858,13 +3826,13 @@
       <c r="E27" t="s">
         <v>92</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27">
         <v>1</v>
       </c>
       <c r="H27" t="s">
         <v>31</v>
       </c>
-      <c r="I27" s="4">
+      <c r="I27">
         <v>1</v>
       </c>
     </row>
@@ -3878,13 +3846,13 @@
       <c r="E28" t="s">
         <v>119</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28">
         <v>1</v>
       </c>
       <c r="H28" t="s">
         <v>11</v>
       </c>
-      <c r="I28" s="4">
+      <c r="I28">
         <v>1</v>
       </c>
     </row>
@@ -3898,13 +3866,13 @@
       <c r="E29" t="s">
         <v>120</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29">
         <v>2</v>
       </c>
       <c r="H29" t="s">
         <v>38</v>
       </c>
-      <c r="I29" s="4">
+      <c r="I29">
         <v>1</v>
       </c>
     </row>
@@ -3918,13 +3886,13 @@
       <c r="E30" t="s">
         <v>75</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30">
         <v>1</v>
       </c>
       <c r="H30" t="s">
         <v>13</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I30">
         <v>1</v>
       </c>
     </row>
@@ -3938,13 +3906,13 @@
       <c r="E31" t="s">
         <v>132</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31">
         <v>1</v>
       </c>
       <c r="H31" t="s">
         <v>30</v>
       </c>
-      <c r="I31" s="4">
+      <c r="I31">
         <v>1</v>
       </c>
     </row>
@@ -3958,13 +3926,13 @@
       <c r="E32" t="s">
         <v>126</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32">
         <v>1</v>
       </c>
       <c r="H32" t="s">
         <v>18</v>
       </c>
-      <c r="I32" s="4">
+      <c r="I32">
         <v>2</v>
       </c>
     </row>
@@ -3978,13 +3946,13 @@
       <c r="E33" t="s">
         <v>95</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33">
         <v>2</v>
       </c>
       <c r="H33" t="s">
         <v>37</v>
       </c>
-      <c r="I33" s="4">
+      <c r="I33">
         <v>1</v>
       </c>
     </row>
@@ -3998,13 +3966,13 @@
       <c r="E34" t="s">
         <v>103</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F34">
         <v>3</v>
       </c>
       <c r="H34" t="s">
         <v>17</v>
       </c>
-      <c r="I34" s="4">
+      <c r="I34">
         <v>1</v>
       </c>
     </row>
@@ -4018,13 +3986,13 @@
       <c r="E35" t="s">
         <v>105</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35">
         <v>1</v>
       </c>
       <c r="H35" t="s">
         <v>16</v>
       </c>
-      <c r="I35" s="4">
+      <c r="I35">
         <v>2</v>
       </c>
     </row>
@@ -4038,13 +4006,13 @@
       <c r="E36" t="s">
         <v>90</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36">
         <v>1</v>
       </c>
       <c r="H36" t="s">
         <v>26</v>
       </c>
-      <c r="I36" s="4">
+      <c r="I36">
         <v>1</v>
       </c>
     </row>
@@ -4058,13 +4026,13 @@
       <c r="E37" t="s">
         <v>108</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37">
         <v>1</v>
       </c>
       <c r="H37" t="s">
         <v>12</v>
       </c>
-      <c r="I37" s="4">
+      <c r="I37">
         <v>1</v>
       </c>
     </row>
@@ -4078,13 +4046,13 @@
       <c r="E38" t="s">
         <v>88</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38">
         <v>1</v>
       </c>
       <c r="H38" t="s">
         <v>10</v>
       </c>
-      <c r="I38" s="4">
+      <c r="I38">
         <v>1</v>
       </c>
     </row>
@@ -4098,13 +4066,13 @@
       <c r="E39" t="s">
         <v>60</v>
       </c>
-      <c r="F39" s="4">
+      <c r="F39">
         <v>1</v>
       </c>
       <c r="H39" t="s">
         <v>33</v>
       </c>
-      <c r="I39" s="4">
+      <c r="I39">
         <v>1</v>
       </c>
     </row>
@@ -4118,13 +4086,13 @@
       <c r="E40" t="s">
         <v>111</v>
       </c>
-      <c r="F40" s="4">
+      <c r="F40">
         <v>3</v>
       </c>
       <c r="H40" t="s">
         <v>29</v>
       </c>
-      <c r="I40" s="4">
+      <c r="I40">
         <v>1</v>
       </c>
     </row>
@@ -4138,13 +4106,13 @@
       <c r="E41" t="s">
         <v>30</v>
       </c>
-      <c r="F41" s="4">
+      <c r="F41">
         <v>1</v>
       </c>
       <c r="H41" t="s">
         <v>50</v>
       </c>
-      <c r="I41" s="4">
+      <c r="I41">
         <v>1</v>
       </c>
     </row>
@@ -4158,13 +4126,13 @@
       <c r="E42" t="s">
         <v>124</v>
       </c>
-      <c r="F42" s="4">
+      <c r="F42">
         <v>2</v>
       </c>
       <c r="H42" t="s">
         <v>42</v>
       </c>
-      <c r="I42" s="4">
+      <c r="I42">
         <v>3</v>
       </c>
     </row>
@@ -4178,13 +4146,13 @@
       <c r="E43" t="s">
         <v>69</v>
       </c>
-      <c r="F43" s="4">
+      <c r="F43">
         <v>2</v>
       </c>
       <c r="H43" t="s">
         <v>35</v>
       </c>
-      <c r="I43" s="4">
+      <c r="I43">
         <v>1</v>
       </c>
     </row>
@@ -4198,13 +4166,13 @@
       <c r="E44" t="s">
         <v>68</v>
       </c>
-      <c r="F44" s="4">
+      <c r="F44">
         <v>2</v>
       </c>
       <c r="H44" t="s">
         <v>19</v>
       </c>
-      <c r="I44" s="4">
+      <c r="I44">
         <v>1</v>
       </c>
     </row>
@@ -4218,13 +4186,13 @@
       <c r="E45" t="s">
         <v>110</v>
       </c>
-      <c r="F45" s="4">
+      <c r="F45">
         <v>3</v>
       </c>
       <c r="H45" t="s">
         <v>6</v>
       </c>
-      <c r="I45" s="4">
+      <c r="I45">
         <v>1</v>
       </c>
     </row>
@@ -4238,13 +4206,13 @@
       <c r="E46" t="s">
         <v>127</v>
       </c>
-      <c r="F46" s="4">
+      <c r="F46">
         <v>1</v>
       </c>
       <c r="H46" t="s">
         <v>49</v>
       </c>
-      <c r="I46" s="4">
+      <c r="I46">
         <v>1</v>
       </c>
     </row>
@@ -4258,13 +4226,13 @@
       <c r="E47" t="s">
         <v>93</v>
       </c>
-      <c r="F47" s="4">
+      <c r="F47">
         <v>1</v>
       </c>
       <c r="H47" t="s">
         <v>28</v>
       </c>
-      <c r="I47" s="4">
+      <c r="I47">
         <v>1</v>
       </c>
     </row>
@@ -4278,13 +4246,13 @@
       <c r="E48" t="s">
         <v>113</v>
       </c>
-      <c r="F48" s="4">
+      <c r="F48">
         <v>1</v>
       </c>
       <c r="H48" t="s">
         <v>40</v>
       </c>
-      <c r="I48" s="4">
+      <c r="I48">
         <v>1</v>
       </c>
     </row>
@@ -4298,13 +4266,13 @@
       <c r="E49" t="s">
         <v>100</v>
       </c>
-      <c r="F49" s="4">
+      <c r="F49">
         <v>2</v>
       </c>
       <c r="H49" t="s">
         <v>21</v>
       </c>
-      <c r="I49" s="4">
+      <c r="I49">
         <v>1</v>
       </c>
     </row>
@@ -4318,13 +4286,13 @@
       <c r="E50" t="s">
         <v>91</v>
       </c>
-      <c r="F50" s="4">
+      <c r="F50">
         <v>1</v>
       </c>
       <c r="H50" t="s">
         <v>138</v>
       </c>
-      <c r="I50" s="4">
+      <c r="I50">
         <v>58</v>
       </c>
     </row>
@@ -4338,7 +4306,7 @@
       <c r="E51" t="s">
         <v>125</v>
       </c>
-      <c r="F51" s="4">
+      <c r="F51">
         <v>1</v>
       </c>
     </row>
@@ -4352,7 +4320,7 @@
       <c r="E52" t="s">
         <v>87</v>
       </c>
-      <c r="F52" s="4">
+      <c r="F52">
         <v>2</v>
       </c>
     </row>
@@ -4366,7 +4334,7 @@
       <c r="E53" t="s">
         <v>64</v>
       </c>
-      <c r="F53" s="4">
+      <c r="F53">
         <v>1</v>
       </c>
     </row>
@@ -4380,7 +4348,7 @@
       <c r="E54" t="s">
         <v>128</v>
       </c>
-      <c r="F54" s="4">
+      <c r="F54">
         <v>1</v>
       </c>
     </row>
@@ -4394,7 +4362,7 @@
       <c r="E55" t="s">
         <v>99</v>
       </c>
-      <c r="F55" s="4">
+      <c r="F55">
         <v>1</v>
       </c>
     </row>
@@ -4408,7 +4376,7 @@
       <c r="E56" t="s">
         <v>71</v>
       </c>
-      <c r="F56" s="4">
+      <c r="F56">
         <v>7</v>
       </c>
     </row>
@@ -4422,7 +4390,7 @@
       <c r="E57" t="s">
         <v>81</v>
       </c>
-      <c r="F57" s="4">
+      <c r="F57">
         <v>5</v>
       </c>
     </row>
@@ -4436,7 +4404,7 @@
       <c r="E58" t="s">
         <v>67</v>
       </c>
-      <c r="F58" s="4">
+      <c r="F58">
         <v>2</v>
       </c>
     </row>
@@ -4450,7 +4418,7 @@
       <c r="E59" t="s">
         <v>115</v>
       </c>
-      <c r="F59" s="4">
+      <c r="F59">
         <v>1</v>
       </c>
     </row>
@@ -4464,7 +4432,7 @@
       <c r="E60" t="s">
         <v>94</v>
       </c>
-      <c r="F60" s="4">
+      <c r="F60">
         <v>2</v>
       </c>
     </row>
@@ -4475,7 +4443,7 @@
       <c r="E61" t="s">
         <v>112</v>
       </c>
-      <c r="F61" s="4">
+      <c r="F61">
         <v>1</v>
       </c>
     </row>
@@ -4486,7 +4454,7 @@
       <c r="E62" t="s">
         <v>117</v>
       </c>
-      <c r="F62" s="4">
+      <c r="F62">
         <v>6</v>
       </c>
     </row>
@@ -4497,7 +4465,7 @@
       <c r="E63" t="s">
         <v>70</v>
       </c>
-      <c r="F63" s="4">
+      <c r="F63">
         <v>1</v>
       </c>
     </row>
@@ -4508,7 +4476,7 @@
       <c r="E64" t="s">
         <v>82</v>
       </c>
-      <c r="F64" s="4">
+      <c r="F64">
         <v>2</v>
       </c>
     </row>
@@ -4519,7 +4487,7 @@
       <c r="E65" t="s">
         <v>65</v>
       </c>
-      <c r="F65" s="4">
+      <c r="F65">
         <v>1</v>
       </c>
     </row>
@@ -4530,7 +4498,7 @@
       <c r="E66" t="s">
         <v>114</v>
       </c>
-      <c r="F66" s="4">
+      <c r="F66">
         <v>1</v>
       </c>
     </row>
@@ -4541,7 +4509,7 @@
       <c r="E67" t="s">
         <v>80</v>
       </c>
-      <c r="F67" s="4">
+      <c r="F67">
         <v>7</v>
       </c>
     </row>
@@ -4552,7 +4520,7 @@
       <c r="E68" t="s">
         <v>104</v>
       </c>
-      <c r="F68" s="4">
+      <c r="F68">
         <v>2</v>
       </c>
     </row>
@@ -4563,7 +4531,7 @@
       <c r="E69" t="s">
         <v>77</v>
       </c>
-      <c r="F69" s="4">
+      <c r="F69">
         <v>5</v>
       </c>
     </row>
@@ -4574,7 +4542,7 @@
       <c r="E70" t="s">
         <v>40</v>
       </c>
-      <c r="F70" s="4">
+      <c r="F70">
         <v>1</v>
       </c>
     </row>
@@ -4585,7 +4553,7 @@
       <c r="E71" t="s">
         <v>73</v>
       </c>
-      <c r="F71" s="4">
+      <c r="F71">
         <v>3</v>
       </c>
     </row>
@@ -4596,7 +4564,7 @@
       <c r="E72" t="s">
         <v>129</v>
       </c>
-      <c r="F72" s="4">
+      <c r="F72">
         <v>1</v>
       </c>
     </row>
@@ -4607,7 +4575,7 @@
       <c r="E73" t="s">
         <v>138</v>
       </c>
-      <c r="F73" s="4">
+      <c r="F73">
         <v>138</v>
       </c>
     </row>

</xml_diff>